<commit_message>
OW-268 refactored slightly MarkiSwapService
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/OneIRS.xlsx
+++ b/valuation-app/src/test/resources/excel/OneIRS.xlsx
@@ -5,12 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="IRS" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="FRA" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="OIS" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="IRS-Cleared" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t xml:space="preserve">Value Date</t>
   </si>
@@ -226,18 +224,6 @@
   </si>
   <si>
     <t xml:space="preserve">J.P. Morgan Securities Australia Limited</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Direction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRA_PAYMENT_DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRA_FIXING_DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Counterpart Firm ID</t>
   </si>
 </sst>
 </file>
@@ -345,54 +331,55 @@
   </sheetPr>
   <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2 A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="38.8775510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.4387755102041"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.484693877551"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="34.2857142857143"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="38.3367346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,300 +659,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AG1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="1" sqref="A2 D16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA1" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB1" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC1" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD1" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE1" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF1" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG1" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AS1"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="33" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="35" style="0" width="8.36734693877551"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="X1" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y1" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA1" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB1" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC1" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="AD1" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="AE1" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="AF1" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG1" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI1" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ1" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="AK1" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL1" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="AM1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN1" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="AO1" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP1" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ1" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="AR1" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS1" s="0" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
OW-268 fixed issue with data format in the excel files by following strata conventions
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/OneIRS.xlsx
+++ b/valuation-app/src/test/resources/excel/OneIRS.xlsx
@@ -190,13 +190,13 @@
     <t xml:space="preserve">6M</t>
   </si>
   <si>
-    <t xml:space="preserve">MODFOLLOWING</t>
+    <t xml:space="preserve">ModifiedFollowing</t>
   </si>
   <si>
     <t xml:space="preserve">AUSY</t>
   </si>
   <si>
-    <t xml:space="preserve">ACT/365.FIXED</t>
+    <t xml:space="preserve">Act/365F</t>
   </si>
   <si>
     <t xml:space="preserve">10,000,000.00</t>
@@ -331,55 +331,54 @@
   </sheetPr>
   <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2 AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.484693877551"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="38.3367346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.47959183673469"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="36.9897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
OW-268 link uploaded trades to their account
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/OneIRS.xlsx
+++ b/valuation-app/src/test/resources/excel/OneIRS.xlsx
@@ -160,7 +160,7 @@
     <t xml:space="preserve">FCM Name</t>
   </si>
   <si>
-    <t xml:space="preserve">MEGA104</t>
+    <t xml:space="preserve">acc1</t>
   </si>
   <si>
     <t xml:space="preserve">AUD</t>
@@ -331,54 +331,55 @@
   </sheetPr>
   <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2 AH2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="32.9387755102041"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="36.9897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="32.530612244898"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
OW-370 changes needed for the new qa.acuo.com instance
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/OneIRS.xlsx
+++ b/valuation-app/src/test/resources/excel/OneIRS.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
   <si>
     <t xml:space="preserve">Value Date</t>
   </si>
@@ -158,9 +158,27 @@
     <t xml:space="preserve">Jurisdiction</t>
   </si>
   <si>
+    <t xml:space="preserve">FCM ID</t>
+  </si>
+  <si>
     <t xml:space="preserve">FCM Name</t>
   </si>
   <si>
+    <t xml:space="preserve">Portfolio ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPVadj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pNPVadj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notionaladj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IM</t>
+  </si>
+  <si>
     <t xml:space="preserve">ACUOSG8745</t>
   </si>
   <si>
@@ -221,10 +239,16 @@
     <t xml:space="preserve">ASX</t>
   </si>
   <si>
-    <t xml:space="preserve">AU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J.P. Morgan Securities Australia Limited</t>
+    <t xml:space="preserve">EU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">549300MHCFARP0SMZV21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goldman Sachs &amp; Co.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p31</t>
   </si>
   <si>
     <t xml:space="preserve">Trade type</t>
@@ -254,7 +278,10 @@
     <t xml:space="preserve">SGD-SOR-Reuters</t>
   </si>
   <si>
-    <t xml:space="preserve">Singapore</t>
+    <t xml:space="preserve">p1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mexico</t>
   </si>
 </sst>
 </file>
@@ -265,7 +292,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -286,11 +313,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -335,16 +357,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -369,57 +387,59 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AT2"/>
+  <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AS1" activeCellId="0" sqref="AS1:AZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="25.6479591836735"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="30.9132653061224"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="45" min="44" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="34.6938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.07142857142857"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.01020408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.54081632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.26020408163265"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.6071428571429"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="13.7959183673469"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.734693877551"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="33.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,13 +581,31 @@
       <c r="AT1" s="0" t="s">
         <v>45</v>
       </c>
+      <c r="AU1" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" s="0" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>41631</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>11811123</v>
@@ -576,7 +614,7 @@
         <v>455123</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>40882</v>
@@ -588,43 +626,43 @@
         <v>41605</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>999</v>
       </c>
       <c r="O2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="P2" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>47</v>
-      </c>
       <c r="R2" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="Y2" s="1" t="n">
         <v>40882</v>
@@ -633,37 +671,37 @@
         <v>43439</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="AC2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="AE2" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="AD2" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="AF2" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="AH2" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="AI2" s="0" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="AK2" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="AL2" s="1" t="n">
         <v>40882</v>
@@ -672,22 +710,41 @@
         <v>43439</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AS2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AT2" s="0" t="s">
-        <v>67</v>
+        <v>71</v>
+      </c>
+      <c r="AS2" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AV2" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW2" s="0" t="n">
+        <v>-631053.94</v>
+      </c>
+      <c r="AX2" s="0" t="n">
+        <v>-621377.18</v>
+      </c>
+      <c r="AY2" s="0" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="AZ2" s="0" t="n">
+        <f aca="false">0.04*AY2</f>
+        <v>400000</v>
       </c>
     </row>
   </sheetData>
@@ -706,55 +763,56 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AP2"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AR1" activeCellId="1" sqref="AS1:AZ2 AR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="6.47959183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.54081632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.2091836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="30.4744897959184"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.4948979591837"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.7142857142857"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.2142857142857"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.5204081632653"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.5765306122449"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.2397959183673"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="16.9897959183673"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="13.2397959183673"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.6785714285714"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -783,7 +841,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>13</v>
@@ -876,13 +934,19 @@
         <v>42</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="AP1" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="AR1" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -890,7 +954,7 @@
         <v>41631</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>11811152</v>
@@ -899,7 +963,7 @@
         <v>455820</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>41607</v>
@@ -911,31 +975,31 @@
         <v>41605</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>999</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="U2" s="1" t="n">
         <v>41607</v>
@@ -944,37 +1008,37 @@
         <v>44164</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="Y2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA2" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="Z2" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>55</v>
-      </c>
       <c r="AB2" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="AG2" s="0" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="AH2" s="1" t="n">
         <v>41607</v>
@@ -983,13 +1047,13 @@
         <v>44164</v>
       </c>
       <c r="AJ2" s="0" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="AN2" s="0" t="n">
         <v>11911171</v>
@@ -998,7 +1062,13 @@
         <v>12011171</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
+      </c>
+      <c r="AQ2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR2" s="0" t="n">
+        <v>10000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OW-453 refactoring to see a bit better whats going on
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/OneIRS.xlsx
+++ b/valuation-app/src/test/resources/excel/OneIRS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IRS-Cleared" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="89">
   <si>
     <t xml:space="preserve">Value Date</t>
   </si>
@@ -182,6 +182,9 @@
     <t xml:space="preserve">ACUOSG8745</t>
   </si>
   <si>
+    <t xml:space="preserve">455123</t>
+  </si>
+  <si>
     <t xml:space="preserve">AUD</t>
   </si>
   <si>
@@ -258,6 +261,9 @@
   </si>
   <si>
     <t xml:space="preserve">Agreement ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">455820</t>
   </si>
   <si>
     <t xml:space="preserve">SGD</t>
@@ -288,9 +294,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -357,12 +364,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -389,57 +400,58 @@
   </sheetPr>
   <dimension ref="A1:AZ2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AS1" activeCellId="0" sqref="AS1:AZ2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.07142857142857"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="6.01020408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.54081632653061"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.26020408163265"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.4948979591837"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.6785714285714"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="19.2142857142857"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.4948979591837"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.6071428571429"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="19.2142857142857"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="13.7959183673469"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.734693877551"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="33.6683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="32.3979591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,7 +464,7 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -601,137 +613,137 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>41631</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>11811123</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>455123</v>
+      <c r="D2" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>40882</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="2" t="n">
         <v>43439</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="2" t="n">
         <v>41605</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>999</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="S2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" s="2" t="n">
+        <v>40882</v>
+      </c>
+      <c r="Z2" s="2" t="n">
+        <v>43439</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE2" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="T2" s="0" t="s">
+      <c r="AF2" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="U2" s="0" t="s">
+      <c r="AG2" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="Y2" s="1" t="n">
+      <c r="AH2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AK2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL2" s="2" t="n">
         <v>40882</v>
       </c>
-      <c r="Z2" s="1" t="n">
+      <c r="AM2" s="2" t="n">
         <v>43439</v>
       </c>
-      <c r="AA2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB2" s="0" t="s">
+      <c r="AN2" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="AC2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI2" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AL2" s="1" t="n">
-        <v>40882</v>
-      </c>
-      <c r="AM2" s="1" t="n">
-        <v>43439</v>
-      </c>
-      <c r="AN2" s="0" t="s">
-        <v>65</v>
-      </c>
       <c r="AP2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AR2" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AS2" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="AT2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AU2" s="2" t="s">
+      <c r="AT2" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="AU2" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="AV2" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="AW2" s="0" t="n">
         <v>-631053.94</v>
@@ -765,54 +777,54 @@
   </sheetPr>
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AE1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AR1" activeCellId="1" sqref="AS1:AZ2 AR1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3214285714286"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.35204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.40816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.79081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="10.0459183673469"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.54081632653061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.2091836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.4948979591837"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.6785714285714"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="19.2142857142857"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.9897959183673"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.8826530612245"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="30.4744897959184"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="19.4948979591837"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.9081632653061"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="19.2142857142857"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="18.5204081632653"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="16.5765306122449"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.2397959183673"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="16.9897959183673"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="13.2397959183673"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.6785714285714"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -825,7 +837,7 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="0" t="s">
@@ -841,7 +853,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J1" s="0" t="s">
         <v>13</v>
@@ -934,10 +946,10 @@
         <v>42</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="AP1" s="0" t="s">
         <v>47</v>
@@ -950,7 +962,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>41631</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -959,101 +971,101 @@
       <c r="C2" s="0" t="n">
         <v>11811152</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>455820</v>
+      <c r="D2" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <v>41607</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="2" t="n">
         <v>44164</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="2" t="n">
         <v>41605</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>999</v>
       </c>
       <c r="K2" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="L2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>79</v>
-      </c>
       <c r="N2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="U2" s="2" t="n">
+        <v>41607</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>44164</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA2" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="U2" s="1" t="n">
+      <c r="AB2" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AE2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH2" s="2" t="n">
         <v>41607</v>
       </c>
-      <c r="V2" s="1" t="n">
+      <c r="AI2" s="2" t="n">
         <v>44164</v>
       </c>
-      <c r="W2" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="X2" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="Y2" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC2" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="AD2" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AG2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="AH2" s="1" t="n">
-        <v>41607</v>
-      </c>
-      <c r="AI2" s="1" t="n">
-        <v>44164</v>
-      </c>
       <c r="AJ2" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AL2" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AN2" s="0" t="n">
         <v>11911171</v>
@@ -1062,10 +1074,10 @@
         <v>12011171</v>
       </c>
       <c r="AP2" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="AQ2" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="AR2" s="0" t="n">
         <v>10000000</v>

</xml_diff>

<commit_message>
OW-453 fix updating trades on portfolio upload
</commit_message>
<xml_diff>
--- a/valuation-app/src/test/resources/excel/OneIRS.xlsx
+++ b/valuation-app/src/test/resources/excel/OneIRS.xlsx
@@ -284,7 +284,7 @@
     <t xml:space="preserve">SGD-SOR-Reuters</t>
   </si>
   <si>
-    <t xml:space="preserve">p1</t>
+    <t xml:space="preserve">p1a</t>
   </si>
   <si>
     <t xml:space="preserve">Mexico</t>
@@ -406,52 +406,50 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="38" min="38" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="39" min="39" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="43" min="42" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="44" min="44" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="45" min="45" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="46" min="46" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="47" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,54 +775,53 @@
   </sheetPr>
   <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AK1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AP2" activeCellId="0" sqref="AP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.58673469387755"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.6275510204082"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.7959183673469"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="34" min="34" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="35" min="35" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="37" min="37" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="39" min="38" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="40" min="40" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="41" min="41" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="42" min="42" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="43" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>